<commit_message>
Add parameters to oversight form
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="121">
   <si>
     <t>name</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>Current date and time</t>
+  </si>
+  <si>
+    <t>rows=xx</t>
+  </si>
+  <si>
+    <t>Number of lines to show when editing a text question, xx shuld be replaced by the number</t>
+  </si>
+  <si>
+    <t>parameters</t>
   </si>
 </sst>
 </file>
@@ -946,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1423,135 +1432,135 @@
       <c r="D50" s="12"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="30">
+    <row r="51" spans="1:5">
       <c r="A51" s="1"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17" t="s">
-        <v>106</v>
-      </c>
+      <c r="B51" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5">
       <c r="A52" s="1"/>
-      <c r="B52" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="B52" s="2"/>
       <c r="C52" s="12" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
-      <c r="B53" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>108</v>
-      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>104</v>
+      <c r="B54" s="16"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" ht="30">
       <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
+      <c r="B55" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C55" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="30">
+    <row r="56" spans="1:5">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="D56" s="12" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1"/>
-      <c r="B57" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12" t="s">
-        <v>111</v>
+      <c r="B57" s="2"/>
+      <c r="C57" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="C58" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" ht="30">
       <c r="A59" s="1"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D59" s="18"/>
+      <c r="B59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
-      <c r="B60" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D60" s="11"/>
+      <c r="B60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="11"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="11"/>
+      <c r="C62" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="18"/>
       <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C63" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="5"/>
@@ -1560,52 +1569,46 @@
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
       <c r="C64" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" ht="30">
+    <row r="65" spans="1:5">
       <c r="A65" s="1"/>
       <c r="B65" s="6"/>
       <c r="C65" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D65" s="11"/>
       <c r="E65" s="5"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>35</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D66" s="11"/>
       <c r="E66" s="5"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>92</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D67" s="11"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" ht="30">
       <c r="A68" s="1"/>
       <c r="B68" s="6"/>
       <c r="C68" s="11" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E68" s="5"/>
     </row>
@@ -1613,10 +1616,10 @@
       <c r="A69" s="1"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>117</v>
+        <v>35</v>
       </c>
       <c r="E69" s="5"/>
     </row>
@@ -1624,10 +1627,10 @@
       <c r="A70" s="1"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E70" s="5"/>
     </row>
@@ -1635,10 +1638,10 @@
       <c r="A71" s="1"/>
       <c r="B71" s="6"/>
       <c r="C71" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="E71" s="5"/>
     </row>
@@ -1646,10 +1649,10 @@
       <c r="A72" s="1"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="E72" s="5"/>
     </row>
@@ -1657,30 +1660,32 @@
       <c r="A73" s="1"/>
       <c r="B73" s="6"/>
       <c r="C73" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73" s="11"/>
+        <v>115</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1"/>
       <c r="B74" s="6"/>
       <c r="C74" s="11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="E74" s="5"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="E75" s="5"/>
     </row>
@@ -1688,38 +1693,69 @@
       <c r="A76" s="1"/>
       <c r="B76" s="6"/>
       <c r="C76" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D76" s="11"/>
       <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1"/>
       <c r="B77" s="6"/>
       <c r="C77" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E77" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1"/>
       <c r="B78" s="6"/>
       <c r="C78" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E78" s="5"/>
+      <c r="E81" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C62:D62"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add referenced questions when editing a managed form record
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
   <si>
     <t>name</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>parameters</t>
+  </si>
+  <si>
+    <t>Use with a row type of column, space separated parameters from the list below</t>
+  </si>
+  <si>
+    <t>Identify a question that will be the source of data for a column</t>
+  </si>
+  <si>
+    <t>source=question</t>
   </si>
 </sst>
 </file>
@@ -489,8 +498,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -587,7 +598,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -607,6 +618,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -626,6 +638,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -955,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,7 +1451,9 @@
         <v>120</v>
       </c>
       <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
+      <c r="D51" s="12" t="s">
+        <v>121</v>
+      </c>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5">
@@ -1455,130 +1470,130 @@
     <row r="53" spans="1:5">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="C53" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="30">
+    <row r="54" spans="1:5">
       <c r="A54" s="1"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="1"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="30">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2" t="s">
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C57" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D57" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>104</v>
       </c>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
+      <c r="B58" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C58" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1"/>
-      <c r="B60" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12" t="s">
-        <v>111</v>
+      <c r="B60" s="2"/>
+      <c r="C60" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>104</v>
       </c>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" ht="30">
       <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
+      <c r="B61" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
+      <c r="D61" s="12" t="s">
+        <v>100</v>
+      </c>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D62" s="18"/>
+      <c r="B62" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1"/>
-      <c r="B63" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="11"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1"/>
       <c r="B64" s="6"/>
-      <c r="C64" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" s="11"/>
+      <c r="C64" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="18"/>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="C65" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="5"/>
@@ -1587,7 +1602,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="6"/>
       <c r="C66" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="5"/>
@@ -1596,41 +1611,37 @@
       <c r="A67" s="1"/>
       <c r="B67" s="6"/>
       <c r="C67" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D67" s="11"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="1:5" ht="30">
+    <row r="68" spans="1:5">
       <c r="A68" s="1"/>
       <c r="B68" s="6"/>
       <c r="C68" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D68" s="11"/>
       <c r="E68" s="5"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1"/>
       <c r="B69" s="6"/>
       <c r="C69" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D69" s="11"/>
       <c r="E69" s="5"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" ht="30">
       <c r="A70" s="1"/>
       <c r="B70" s="6"/>
       <c r="C70" s="11" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E70" s="5"/>
     </row>
@@ -1638,10 +1649,10 @@
       <c r="A71" s="1"/>
       <c r="B71" s="6"/>
       <c r="C71" s="11" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E71" s="5"/>
     </row>
@@ -1649,10 +1660,10 @@
       <c r="A72" s="1"/>
       <c r="B72" s="6"/>
       <c r="C72" s="11" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="E72" s="5"/>
     </row>
@@ -1660,10 +1671,10 @@
       <c r="A73" s="1"/>
       <c r="B73" s="6"/>
       <c r="C73" s="11" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="E73" s="5"/>
     </row>
@@ -1671,10 +1682,10 @@
       <c r="A74" s="1"/>
       <c r="B74" s="6"/>
       <c r="C74" s="11" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="E74" s="5"/>
     </row>
@@ -1682,10 +1693,10 @@
       <c r="A75" s="1"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="E75" s="5"/>
     </row>
@@ -1693,52 +1704,52 @@
       <c r="A76" s="1"/>
       <c r="B76" s="6"/>
       <c r="C76" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D76" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1"/>
       <c r="B77" s="6"/>
       <c r="C77" s="11" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E77" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E77" s="5"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1"/>
       <c r="B78" s="6"/>
       <c r="C78" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>79</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D78" s="11"/>
       <c r="E78" s="5"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1"/>
       <c r="B79" s="6"/>
       <c r="C79" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E79" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1"/>
       <c r="B80" s="6"/>
       <c r="C80" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E80" s="5"/>
     </row>
@@ -1746,16 +1757,38 @@
       <c r="A81" s="1"/>
       <c r="B81" s="6"/>
       <c r="C81" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="D83" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E81" s="5"/>
+      <c r="E83" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C64:D64"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add export of parameters when exporting oversight definition
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>source=question</t>
+  </si>
+  <si>
+    <t>auto=yes</t>
+  </si>
+  <si>
+    <t>Use when the source question is of type image, this will identify objects within the image to add as labels</t>
   </si>
 </sst>
 </file>
@@ -970,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1478,11 +1484,15 @@
       </c>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" ht="30">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+      <c r="C54" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5">
@@ -1804,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1869,7 +1879,9 @@
       <c r="O1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="P1"/>
+      <c r="P1" s="4" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2"/>

</xml_diff>

<commit_message>
Add interval arithmetic to filters
</commit_message>
<xml_diff>
--- a/smapServer/WebContent/oversight_template.xlsx
+++ b/smapServer/WebContent/oversight_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>name</t>
   </si>
@@ -386,12 +386,6 @@
     <t>All of the following tokens should be separated by spaces. For example ( 100 + 5 ) / 10</t>
   </si>
   <si>
-    <t>+ integer {nn}</t>
-  </si>
-  <si>
-    <t>Adds nn days to a date.  nn being an integer value</t>
-  </si>
-  <si>
     <t>current_date</t>
   </si>
   <si>
@@ -423,6 +417,60 @@
   </si>
   <si>
     <t>Use when the source question is of type image, this will identify objects within the image to add as labels</t>
+  </si>
+  <si>
+    <t>{1_day}</t>
+  </si>
+  <si>
+    <t>(n_days}</t>
+  </si>
+  <si>
+    <t>{1_hour}</t>
+  </si>
+  <si>
+    <t>{n_hours}</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 day</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n days</t>
+  </si>
+  <si>
+    <t>{1_minute}</t>
+  </si>
+  <si>
+    <t>{n_minutes}</t>
+  </si>
+  <si>
+    <t>{1_second}</t>
+  </si>
+  <si>
+    <t>{n_seconds}</t>
+  </si>
+  <si>
+    <t>{hh:mm:ss}</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time byhh hours mm minutes and ss seconds</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n seconds</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1second</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n minutes</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 minute</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by n hours</t>
+  </si>
+  <si>
+    <t>Modifies a date/ date time by 1 hour</t>
   </si>
 </sst>
 </file>
@@ -504,8 +552,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -608,7 +670,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -631,6 +693,13 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +722,13 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -982,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1462,11 +1538,11 @@
     <row r="51" spans="1:5">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E51" s="5"/>
     </row>
@@ -1474,10 +1550,10 @@
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E52" s="5"/>
     </row>
@@ -1485,10 +1561,10 @@
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E53" s="5"/>
     </row>
@@ -1496,10 +1572,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E54" s="5"/>
     </row>
@@ -1703,7 +1779,7 @@
         <v>38</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E74" s="5"/>
     </row>
@@ -1711,10 +1787,10 @@
       <c r="A75" s="1"/>
       <c r="B75" s="6"/>
       <c r="C75" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E75" s="5"/>
     </row>
@@ -1794,15 +1870,85 @@
       <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="1"/>
       <c r="B83" s="6"/>
       <c r="C83" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="E83" s="5"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="B84" s="6"/>
+      <c r="C84" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="B85" s="6"/>
+      <c r="C85" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="B86" s="6"/>
+      <c r="C86" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="B87" s="6"/>
+      <c r="C87" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="B88" s="6"/>
+      <c r="C88" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="B89" s="6"/>
+      <c r="C89" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="B90" s="6"/>
+      <c r="C90" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91" s="6"/>
+      <c r="C91" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>135</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1822,7 +1968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1886,7 +2032,7 @@
         <v>110</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -2723,7 +2869,7 @@
         <v>110</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:21">

</xml_diff>